<commit_message>
added number line integers simulation
</commit_message>
<xml_diff>
--- a/html-simulations.xlsx
+++ b/html-simulations.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test\trunk\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="80" windowWidth="20120" windowHeight="8000"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="68">
   <si>
     <t>SNO</t>
   </si>
@@ -210,12 +205,27 @@
   </si>
   <si>
     <t>equations</t>
+  </si>
+  <si>
+    <t>number line integres</t>
+  </si>
+  <si>
+    <t>birds</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>generic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -307,7 +317,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,7 +352,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -551,22 +561,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.81640625" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -1013,6 +1023,32 @@
         <v>62</v>
       </c>
       <c r="I21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" t="s">
+        <v>67</v>
+      </c>
+      <c r="I22" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1027,7 +1063,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1039,7 +1075,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Energy forms and changes, graphing lines splited as individual pages
</commit_message>
<xml_diff>
--- a/html-simulations.xlsx
+++ b/html-simulations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
   <si>
     <t>SNO</t>
   </si>
@@ -220,6 +220,27 @@
   </si>
   <si>
     <t>generic</t>
+  </si>
+  <si>
+    <t>graphing-lines</t>
+  </si>
+  <si>
+    <t>energy-forms-and-changes</t>
+  </si>
+  <si>
+    <t>systems</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>slope-intercept</t>
+  </si>
+  <si>
+    <t>point-slope</t>
+  </si>
+  <si>
+    <t>line-game</t>
   </si>
 </sst>
 </file>
@@ -561,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +593,7 @@
     <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -1049,6 +1070,52 @@
         <v>67</v>
       </c>
       <c r="I22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+      <c r="I24" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>